<commit_message>
xong ly thuey 1-8
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Hime Ichimaru</t>
+  </si>
+  <si>
+    <t>Anal</t>
+  </si>
+  <si>
+    <t>https://jav.la/video/47578/mukd-452-jav-streaming-anal-anal-sex-for-the-first-time-when-i-was-born-the-last-day-of-virginityand-the-first-anal-anal-fucking-out-yuka-shirai-yukari.html</t>
   </si>
 </sst>
 </file>
@@ -450,288 +456,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
-    <hyperlink ref="B9" r:id="rId4" tooltip="Marina Yuzuki" display="https://bestjavporn.com/pornstar/marina-yuzuki/"/>
-    <hyperlink ref="C8" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6" tooltip="Maina Yuri" display="https://bestjavporn.com/pornstar/maina-yuri/"/>
-    <hyperlink ref="C10" r:id="rId7"/>
-    <hyperlink ref="C14" r:id="rId8"/>
-    <hyperlink ref="C16" r:id="rId9"/>
-    <hyperlink ref="C17" r:id="rId10"/>
-    <hyperlink ref="C18" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12" tooltip="Nene Tanaka" display="https://bestjavporn.com/pornstar/nene-tanaka/"/>
-    <hyperlink ref="B21" r:id="rId13" tooltip="Aimi Irie" display="https://bestjavporn.com/pornstar/aimi-irie/"/>
-    <hyperlink ref="C21" r:id="rId14"/>
-    <hyperlink ref="B22" r:id="rId15" tooltip="Cocoa Aisu" display="https://bestjavporn.com/pornstar/cocoa-aisu/"/>
-    <hyperlink ref="C13" r:id="rId16"/>
-    <hyperlink ref="C24" r:id="rId17"/>
-    <hyperlink ref="B24" r:id="rId18" tooltip="Waka Misono" display="https://bestjavporn.com/pornstar/waka-misono/"/>
-    <hyperlink ref="C27" r:id="rId19"/>
-    <hyperlink ref="B27" r:id="rId20" tooltip="Hime Ichimaru" display="https://bestjavporn.com/pornstar/hime-ichimaru/"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="C9" r:id="rId4" tooltip="Marina Yuzuki" display="https://bestjavporn.com/pornstar/marina-yuzuki/"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="C10" r:id="rId6" tooltip="Maina Yuri" display="https://bestjavporn.com/pornstar/maina-yuri/"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D14" r:id="rId8"/>
+    <hyperlink ref="D16" r:id="rId9"/>
+    <hyperlink ref="D17" r:id="rId10"/>
+    <hyperlink ref="D18" r:id="rId11"/>
+    <hyperlink ref="C16" r:id="rId12" tooltip="Nene Tanaka" display="https://bestjavporn.com/pornstar/nene-tanaka/"/>
+    <hyperlink ref="C21" r:id="rId13" tooltip="Aimi Irie" display="https://bestjavporn.com/pornstar/aimi-irie/"/>
+    <hyperlink ref="D21" r:id="rId14"/>
+    <hyperlink ref="C22" r:id="rId15" tooltip="Cocoa Aisu" display="https://bestjavporn.com/pornstar/cocoa-aisu/"/>
+    <hyperlink ref="D13" r:id="rId16"/>
+    <hyperlink ref="D24" r:id="rId17"/>
+    <hyperlink ref="C24" r:id="rId18" tooltip="Waka Misono" display="https://bestjavporn.com/pornstar/waka-misono/"/>
+    <hyperlink ref="D27" r:id="rId19"/>
+    <hyperlink ref="C27" r:id="rId20" tooltip="Hime Ichimaru" display="https://bestjavporn.com/pornstar/hime-ichimaru/"/>
+    <hyperlink ref="D29" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>